<commit_message>
estadistica semana del 15 de enero
</commit_message>
<xml_diff>
--- a/cambios_de_estado_de_cita.xlsx
+++ b/cambios_de_estado_de_cita.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositorios\estadistica_agendamientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\estadistica_agendamientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C089C5F4-8075-4DD2-8F64-F8A4C1DAEA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727D007D-D5F4-49B8-94E8-FB33E8FC53DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10920" yWindow="2112" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>15_01_2024</t>
+  </si>
+  <si>
+    <t>21_01_2024</t>
   </si>
 </sst>
 </file>
@@ -366,20 +369,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,8 +395,11 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -406,8 +412,11 @@
       <c r="D2">
         <v>2525</v>
       </c>
+      <c r="E2">
+        <v>2638</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -420,8 +429,11 @@
       <c r="D3">
         <v>1910</v>
       </c>
+      <c r="E3">
+        <v>2032</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -434,8 +446,11 @@
       <c r="D4">
         <v>3373</v>
       </c>
+      <c r="E4">
+        <v>3446</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -447,6 +462,9 @@
       </c>
       <c r="D5">
         <v>6704</v>
+      </c>
+      <c r="E5">
+        <v>6784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregados los datos de semana de lunes 22 de enero
</commit_message>
<xml_diff>
--- a/cambios_de_estado_de_cita.xlsx
+++ b/cambios_de_estado_de_cita.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\estadistica_agendamientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositorios\estadistica_agendamientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727D007D-D5F4-49B8-94E8-FB33E8FC53DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8000016-7F8D-4C29-85F6-4BE0CB16BB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>21_01_2024</t>
+  </si>
+  <si>
+    <t>28_01_2024</t>
   </si>
 </sst>
 </file>
@@ -369,20 +372,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,8 +401,11 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -415,8 +421,11 @@
       <c r="E2">
         <v>2638</v>
       </c>
+      <c r="F2">
+        <v>2824</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -432,8 +441,11 @@
       <c r="E3">
         <v>2032</v>
       </c>
+      <c r="F3">
+        <v>2097</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -449,8 +461,11 @@
       <c r="E4">
         <v>3446</v>
       </c>
+      <c r="F4">
+        <v>3537</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -465,6 +480,9 @@
       </c>
       <c r="E5">
         <v>6784</v>
+      </c>
+      <c r="F5">
+        <v>6858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregan los datos desde el lunes 29 de enero hasta el miercoles 7 de febrero
</commit_message>
<xml_diff>
--- a/cambios_de_estado_de_cita.xlsx
+++ b/cambios_de_estado_de_cita.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositorios\estadistica_agendamientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8000016-7F8D-4C29-85F6-4BE0CB16BB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D9D17A-0370-43E2-BCA8-80D19811B079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>28_01_2024</t>
+  </si>
+  <si>
+    <t>07_02_2024</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,7 +388,7 @@
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +407,11 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -424,8 +430,11 @@
       <c r="F2">
         <v>2824</v>
       </c>
+      <c r="G2">
+        <v>3063</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -444,8 +453,11 @@
       <c r="F3">
         <v>2097</v>
       </c>
+      <c r="G3">
+        <v>2314</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -464,8 +476,11 @@
       <c r="F4">
         <v>3537</v>
       </c>
+      <c r="G4">
+        <v>3618</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -483,6 +498,9 @@
       </c>
       <c r="F5">
         <v>6858</v>
+      </c>
+      <c r="G5">
+        <v>6927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>